<commit_message>
fixed some errors in the spreadsheet
</commit_message>
<xml_diff>
--- a/Movement2 Cases.xlsx
+++ b/Movement2 Cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DesmenH_RedSpecter\Source\Repos\FireEscape\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7146BF44-63F6-4A8A-B8B5-C6CB98301DD5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E36C4729-D407-47E7-9FF4-157D39B39530}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4890" yWindow="1230" windowWidth="31020" windowHeight="15780" xr2:uid="{D9798590-3DAD-4965-91AE-6043DDDB57F5}"/>
+    <workbookView xWindow="3825" yWindow="705" windowWidth="13545" windowHeight="15780" xr2:uid="{D9798590-3DAD-4965-91AE-6043DDDB57F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -132,9 +132,6 @@
     <t>Stop at end block  |   Elevation + 1</t>
   </si>
   <si>
-    <t>Change fire state + 1  | Stop at middle block  |  Elevation +  1</t>
-  </si>
-  <si>
     <t>Stop at end block  |  Elevation + 1</t>
   </si>
   <si>
@@ -145,6 +142,9 @@
   </si>
   <si>
     <t>Stop at end block | Elevation + 1</t>
+  </si>
+  <si>
+    <t>Change fire state + 1  | Stop at end block  |  Elevation +  1</t>
   </si>
 </sst>
 </file>
@@ -653,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3933FD6F-3E8D-4F2F-912D-F0D01161BCD2}">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -930,7 +930,7 @@
         <v>11</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1018,7 +1018,7 @@
         <v>11</v>
       </c>
       <c r="I17" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1116,7 +1116,7 @@
         <v>11</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1144,7 +1144,7 @@
         <v>15</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1180,7 +1180,7 @@
         <v>11</v>
       </c>
       <c r="I26" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>